<commit_message>
eq conc calc code cleared off series
</commit_message>
<xml_diff>
--- a/input/calorimetry/test_1.xlsx
+++ b/input/calorimetry/test_1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0614B71-3E4E-42BD-B8B3-4BFB9BDB1180}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -20,17 +21,35 @@
     <sheet name="targets" sheetId="6" r:id="rId6"/>
     <sheet name="enthalpies" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+  <si>
+    <t>PLP</t>
+  </si>
+  <si>
+    <t>T3H</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Comp</t>
+  </si>
   <si>
     <t>lg_k</t>
   </si>
@@ -38,30 +57,21 @@
     <t>tot</t>
   </si>
   <si>
-    <t>PLP</t>
-  </si>
-  <si>
-    <t>T3H</t>
-  </si>
-  <si>
     <t>data</t>
   </si>
   <si>
+    <t>volumes</t>
+  </si>
+  <si>
     <t>observation</t>
   </si>
   <si>
+    <t>dilution</t>
+  </si>
+  <si>
     <t>deviation</t>
   </si>
   <si>
-    <t>dilution</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>Comp</t>
-  </si>
-  <si>
     <t xml:space="preserve">constants </t>
   </si>
   <si>
@@ -69,19 +79,16 @@
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>volumes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,27 +400,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -421,7 +428,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -430,21 +437,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
       <c r="A2">
         <v>5.13</v>
       </c>
@@ -455,32 +462,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>7.9702199999999999E-4</v>
       </c>
@@ -490,7 +497,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>7.9569599914063212E-4</v>
       </c>
@@ -500,7 +507,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>7.9437440307285171E-4</v>
       </c>
@@ -510,7 +517,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>7.930571898848895E-4</v>
       </c>
@@ -520,7 +527,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>7.9174433781006978E-4</v>
       </c>
@@ -530,7 +537,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>7.9043582522561173E-4</v>
       </c>
@@ -540,7 +547,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7.8913163065144241E-4</v>
       </c>
@@ -550,7 +557,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>7.8783173274902054E-4</v>
       </c>
@@ -560,7 +567,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>7.8653611032017423E-4</v>
       </c>
@@ -570,7 +577,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>7.852447423059469E-4</v>
       </c>
@@ -580,7 +587,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>7.8395760778545798E-4</v>
       </c>
@@ -590,7 +597,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>7.8267468597477169E-4</v>
       </c>
@@ -598,7 +605,7 @@
         <v>1.0725086253868829E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>7.8139595622577938E-4</v>
       </c>
@@ -606,7 +613,7 @@
         <v>1.1680978543478924E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>7.8012139802509123E-4</v>
       </c>
@@ -614,7 +621,7 @@
         <v>1.2633752464361898E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>7.788509909929395E-4</v>
       </c>
@@ -622,7 +629,7 @@
         <v>1.3583423251060359E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>7.7758471488209233E-4</v>
       </c>
@@ -636,18 +643,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -656,18 +663,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -714,10 +721,13 @@
       <c r="P1">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>15</v>
@@ -764,110 +774,119 @@
       <c r="P2">
         <v>15.349958000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2">
+        <v>15.374955</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>6.9950999999999999E-2</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>6.9513000000000005E-2</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>6.9853999999999999E-2</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>7.1473999999999996E-2</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>6.7108000000000001E-2</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>6.6289000000000001E-2</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>5.6025999999999999E-2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>4.4492999999999998E-2</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2.7882000000000001E-2</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>9.2390000000000007E-3</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>3.0569999999999998E-3</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>2.4859999999999999E-3</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>9.0600000000000001E-4</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>-1.8940000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>-1.9535379999999999E-3</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2.471029E-3</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>-1.7689E-4</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>5.5665399999999996E-4</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>7.0772999999999995E-4</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1.854236E-3</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>1.081072E-3</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>4.7312199999999997E-4</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.06313E-3</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>2.7179899999999998E-4</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>1.168423E-3</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>2.32129E-4</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>9.1735299999999998E-4</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>1.2699580000000001E-3</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>-3.97241E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>9.9999999999999995E-7</v>
@@ -912,6 +931,9 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="P5">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="Q5">
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
@@ -921,21 +943,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -944,29 +966,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>47200</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
postproc and writing added
</commit_message>
<xml_diff>
--- a/input/calorimetry/test_1.xlsx
+++ b/input/calorimetry/test_1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KEVreplica\input\calorimetry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C0A8781-5703-4EF0-A719-1754C943757F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -20,8 +19,9 @@
     <sheet name="heats" sheetId="5" r:id="rId5"/>
     <sheet name="targets" sheetId="6" r:id="rId6"/>
     <sheet name="enthalpies" sheetId="7" r:id="rId7"/>
+    <sheet name="setup" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>PLP</t>
   </si>
@@ -79,16 +79,25 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Calorimeter</t>
+  </si>
+  <si>
+    <t>DSC</t>
+  </si>
+  <si>
+    <t>Initial volume</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,16 +409,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +429,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -437,23 +446,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5.13</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -462,16 +471,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -479,7 +488,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -487,7 +496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>7.9702199999999999E-4</v>
       </c>
@@ -497,7 +506,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>7.9569599914063212E-4</v>
       </c>
@@ -507,7 +516,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>7.9437440307285171E-4</v>
       </c>
@@ -517,7 +526,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>7.930571898848895E-4</v>
       </c>
@@ -527,7 +536,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>7.9174433781006978E-4</v>
       </c>
@@ -537,7 +546,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7.9043582522561173E-4</v>
       </c>
@@ -547,7 +556,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7.8913163065144241E-4</v>
       </c>
@@ -557,7 +566,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7.8783173274902054E-4</v>
       </c>
@@ -567,7 +576,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>7.8653611032017423E-4</v>
       </c>
@@ -577,7 +586,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7.852447423059469E-4</v>
       </c>
@@ -587,7 +596,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>7.8395760778545798E-4</v>
       </c>
@@ -597,7 +606,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7.8267468597477169E-4</v>
       </c>
@@ -605,7 +614,7 @@
         <v>1.0725086253868829E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7.8139595622577938E-4</v>
       </c>
@@ -613,7 +622,7 @@
         <v>1.1680978543478924E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7.8012139802509123E-4</v>
       </c>
@@ -621,7 +630,7 @@
         <v>1.2633752464361898E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7.788509909929395E-4</v>
       </c>
@@ -629,7 +638,7 @@
         <v>1.3583423251060359E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7.7758471488209233E-4</v>
       </c>
@@ -643,16 +652,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -663,16 +672,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -722,7 +731,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -772,7 +781,7 @@
         <v>15.374955</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -822,7 +831,7 @@
         <v>-1.8940000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -872,7 +881,7 @@
         <v>-3.97241E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -928,16 +937,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -951,21 +960,52 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
additional F_min expressions tested
</commit_message>
<xml_diff>
--- a/input/calorimetry/test_1.xlsx
+++ b/input/calorimetry/test_1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="input_stoich_coefficients" sheetId="1" r:id="rId1"/>
@@ -39,18 +39,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
-    <t>PLP</t>
-  </si>
-  <si>
-    <t>T3H</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
-    <t>Comp</t>
-  </si>
-  <si>
     <t>lg_k</t>
   </si>
   <si>
@@ -88,6 +79,15 @@
   </si>
   <si>
     <t>Initial volume</t>
+  </si>
+  <si>
+    <t>Ald</t>
+  </si>
+  <si>
+    <t>Hydr</t>
+  </si>
+  <si>
+    <t>Hydrz</t>
   </si>
 </sst>
 </file>
@@ -413,20 +413,20 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -437,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -449,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -457,7 +457,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -475,25 +475,25 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -656,14 +656,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -676,14 +676,14 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:P1"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -733,57 +733,57 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>15.024997000000001</v>
+        <v>15.024977</v>
       </c>
       <c r="C2">
-        <v>15.049994</v>
+        <v>15.049954</v>
       </c>
       <c r="D2">
-        <v>15.074991000000001</v>
+        <v>15.074930999999999</v>
       </c>
       <c r="E2">
-        <v>15.099988</v>
+        <v>15.099907999999999</v>
       </c>
       <c r="F2">
-        <v>15.124985000000001</v>
+        <v>15.124885000000001</v>
       </c>
       <c r="G2">
-        <v>15.149982</v>
+        <v>15.149862000000001</v>
       </c>
       <c r="H2">
-        <v>15.174979</v>
+        <v>15.174839</v>
       </c>
       <c r="I2">
-        <v>15.199975999999999</v>
+        <v>15.199816</v>
       </c>
       <c r="J2">
-        <v>15.224973</v>
+        <v>15.224793</v>
       </c>
       <c r="K2">
-        <v>15.249969999999999</v>
+        <v>15.24977</v>
       </c>
       <c r="L2">
-        <v>15.274967</v>
+        <v>15.274747</v>
       </c>
       <c r="M2">
-        <v>15.299963999999999</v>
+        <v>15.299723999999999</v>
       </c>
       <c r="N2">
-        <v>15.324961</v>
+        <v>15.324700999999999</v>
       </c>
       <c r="O2">
-        <v>15.349958000000001</v>
+        <v>15.349678000000001</v>
       </c>
       <c r="P2">
-        <v>15.374955</v>
+        <v>15.374655000000001</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>6.9950999999999999E-2</v>
@@ -833,7 +833,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>-1.9535379999999999E-3</v>
@@ -883,7 +883,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>9.9999999999999995E-7</v>
@@ -941,17 +941,17 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -963,7 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -971,10 +971,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -994,15 +994,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>15</v>

</xml_diff>